<commit_message>
add the qrcode ID reader
</commit_message>
<xml_diff>
--- a/SlipReader2/output.xlsx
+++ b/SlipReader2/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>date</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>qr_code_text</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -536,6 +541,11 @@
           <t>16 มิ.ย. 68, 19:26</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>004600060000010103002022520250616192655230052935085102TH91045015</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -588,6 +598,11 @@
           <t>06 เม.ย. 68, 12:32</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>004600060000010103002022520250406123215230058366085102TH91040A46</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -602,42 +617,47 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>นาย อดิเทพ แบบเหมือน</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธนาคารออมสิน</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0204xxxx1195</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>. นายสัญญา ศรีวรรณ.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>พร้อมเพย์</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3909xxxxx4703</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>25.00</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15ก.ค. 2568 17:32</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0045000600000101030300224519617039587I000007B97905102TH9104D7A2</t>
         </is>
       </c>
     </row>
@@ -654,42 +674,47 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ซิลมีย์ ป.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธนาคารกสิกรไทย</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>xxx-x-x2730-x</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ภักดิพระสามารถ ธ.กสิกรไทย</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธ.กสิกรไทย</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>xxx-x-x5833-x</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>14,000.00</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>19 เม.ย. 68 18:07 น.</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0041000600000101030040220015109180730BTF085585102TH91042F11</t>
         </is>
       </c>
     </row>
@@ -706,49 +731,54 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ซิลมีย์ ป.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธนาคารกสิกรไทย</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>xxx-x-x2730-x</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ซิลมีย์ ปะหนัน</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธ.กสิกรไทย</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>xxx-x-x6833-x</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2,000.00</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>30 พ.ค. 68 06:03 น.</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0041000600000101030040220015150060303ATF010635102TH91047FF0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KB.txt</t>
+          <t>K+kitty.txt</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -758,250 +788,389 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ภักดิพรส ธ.กสิกรไทย</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธนาคารกสิกรไทย</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>x-x5833-x</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ภักดิพร สามารถ</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธ.กสิกรไทย</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>xxx-x-x3478-x</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.84</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>16 ก.ค. 68  23:14 น.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0041000600000101030040220015197231427CTF016705102TH9104D930</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KTB.txt</t>
+          <t>K+snoopy.txt</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>krungthai</t>
+          <t>kbank</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ไม่พบชื่อผู้โอน</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธนาคารกสิกรไทย</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>xxx-x-x5833-x</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ไม่พบชื่อผู้รับ</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ไม่พบชื่อธนาคารผู้รับ</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ไม่พบเลขบัญชีผู้รับ</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3,325.00</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ไม่พบวันที่</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0041000600000101030040220015195192032APM136485102TH91041E3C</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mymoo.txt</t>
+          <t>KB.txt</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>gsb</t>
+          <t>kbank</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ซิลมีย์ ป.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธนาคารกสิกรไทย</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>xxx-x-x2730-x</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ภักดิพระสามารถ ธ.กสิกรไทย</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ธ.กสิกรไทย</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>xxx-x-x5833-x</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>14,000.00</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>19 เม.ย. 68 18:07 น.</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0041000600000101030040220015109180730BTF085585102TH91042F11</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SCB.txt</t>
+          <t>KTB.txt</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>scb</t>
+          <t>krungthai</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ซิลมีย์</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>กรุงไทย</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>x-xx882-2</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>น.ส. ซิลมีย์ ปะหนัน</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>กสิกรไทย</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>x-xx833-8</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>500.00</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>20 ก.พ. 2568 15:19</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0038000600000101030060217A78990c2774ba4b195102TH91045737</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Mymoo.txt</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>gsb</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>นาย อดิเทพ แบบเหมือน</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ธนาคารออมสิน</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0204xxxx1195</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>นาย อัฟเฟนดีย์สาอิ</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>เติมเงินพร้อมเพย์</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>4999xxxxx0649</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>15ก.ค. 2568 17:59</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0045000600000101030300224519617054995I000007B97905102TH910450FA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SCB.txt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>scb</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>นางสาว ซิลมีย์ ปะหนัน</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ไทยพาณิชย์</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>xxx xxx189-6</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>น.ส.ศิริวรรณ หมะหวังเอียด</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>ไม่ระบุ</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>xxx xxx-9283</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>25 มิ.ย. 2568 17:53</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0046000600000101030140225202506258EWX6Ejo07FyhP4ev5102TH91048888</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>SCB3500.txt</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>scb</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>นางสาว ซิลมีย์ ปะหนัน</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ไทยพาณิชย์</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>x482</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>น.ส. ซิลมีย์ ปะหนัน</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>ไม่ระบุ</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>x-8338</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>3,500.00</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>01 ก.ค. 2568 10:15</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0046000600000101030140225202507018x482jp7EtCLE2oY15102TH9104F5B4</t>
         </is>
       </c>
     </row>

</xml_diff>